<commit_message>
Peer review in 3 columns. Fixed sudden overlapping of 'with' entries following https://tex.stackexchange.com/a/460754/229974
</commit_message>
<xml_diff>
--- a/data/grant_en.xlsx
+++ b/data/grant_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66262B19-AE54-466A-8684-5E11422CDE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD23197-D651-4FB3-BEFA-9F00F430637C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>what</t>
   </si>
@@ -89,6 +89,21 @@
   </si>
   <si>
     <t>Project: Effects of hormone levels, masculinity and femininity, on pitch discrimination in men and women</t>
+  </si>
+  <si>
+    <t>COP\$89.979.750</t>
+  </si>
+  <si>
+    <t>XI \href{https://www.unbosque.edu.co/investigaciones/convocatorias-investigacion}{Internal Call for Financing Research and Technological Innovation Projects El Bosque University}, 2023</t>
+  </si>
+  <si>
+    <t>Project: \textit{Effect of real and simulated resource control on androphilic women's preferences for masculinity in men's faces: an experimental study using eye-tracking}</t>
+  </si>
+  <si>
+    <t>PI: \href{https://www.researchgate.net/profile/Milena-Vasquez-Amezquita}{Milena Vásquez-Amézquita}</t>
+  </si>
+  <si>
+    <t>Feb. 2024 - Present</t>
   </si>
 </sst>
 </file>
@@ -642,9 +657,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -682,7 +697,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -788,7 +803,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -930,7 +945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -938,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,21 +985,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -992,86 +1007,86 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,21 +1094,35 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -1221,6 +1250,27 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Peer review in 3 columns. Fixed sudden overlapping of 'with' entries following https://tex.stackexchange.com/a/447878/229974
</commit_message>
<xml_diff>
--- a/data/grant_en.xlsx
+++ b/data/grant_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66262B19-AE54-466A-8684-5E11422CDE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD23197-D651-4FB3-BEFA-9F00F430637C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>what</t>
   </si>
@@ -89,6 +89,21 @@
   </si>
   <si>
     <t>Project: Effects of hormone levels, masculinity and femininity, on pitch discrimination in men and women</t>
+  </si>
+  <si>
+    <t>COP\$89.979.750</t>
+  </si>
+  <si>
+    <t>XI \href{https://www.unbosque.edu.co/investigaciones/convocatorias-investigacion}{Internal Call for Financing Research and Technological Innovation Projects El Bosque University}, 2023</t>
+  </si>
+  <si>
+    <t>Project: \textit{Effect of real and simulated resource control on androphilic women's preferences for masculinity in men's faces: an experimental study using eye-tracking}</t>
+  </si>
+  <si>
+    <t>PI: \href{https://www.researchgate.net/profile/Milena-Vasquez-Amezquita}{Milena Vásquez-Amézquita}</t>
+  </si>
+  <si>
+    <t>Feb. 2024 - Present</t>
   </si>
 </sst>
 </file>
@@ -642,9 +657,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -682,7 +697,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -788,7 +803,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -930,7 +945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -938,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,21 +985,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -992,86 +1007,86 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,21 +1094,35 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -1221,6 +1250,27 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>